<commit_message>
Resolved a bug on date, excel was to blame. Should improve resilience.
</commit_message>
<xml_diff>
--- a/app/code/data/examples/example_expenses_en.xlsx
+++ b/app/code/data/examples/example_expenses_en.xlsx
@@ -15,10 +15,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1627831651" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1627831651" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1627831651" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1627831651"/>
+      <pm:revision xmlns:pm="smNativeData" day="1627834486" val="980" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1627834486" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1627834486" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1627834486"/>
     </ext>
   </extLst>
 </workbook>
@@ -1249,7 +1249,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="14">
+  <numFmts count="9">
     <numFmt numFmtId="5" formatCode="#,##0\ &quot;€&quot;;\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
@@ -1258,12 +1258,7 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;\ _€_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="20" formatCode="h:mm"/>
-    <numFmt numFmtId="11" formatCode="0.00E+00"/>
-    <numFmt numFmtId="14" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY;@"/>
+    <numFmt numFmtId="164" formatCode="DD/MM/YYYY;@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -1273,7 +1268,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1627831651" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1627834486" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -1288,7 +1283,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1627831651" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1627834486" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -1304,7 +1299,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1627831651" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1627834486" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -1319,7 +1314,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1627831651" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1627834486" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="240" lang="default"/>
             <pm:ea face="Basic Roman" sz="240" lang="default"/>
@@ -1376,7 +1371,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1627831651"/>
+          <pm:border xmlns:pm="smNativeData" id="1627834486"/>
         </ext>
       </extLst>
     </border>
@@ -1395,7 +1390,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1627831651">
+          <pm:border xmlns:pm="smNativeData" id="1627834486">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1416,7 +1411,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1627831651">
+          <pm:border xmlns:pm="smNativeData" id="1627834486">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1438,7 +1433,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1627831651">
+          <pm:border xmlns:pm="smNativeData" id="1627834486">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1459,7 +1454,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1627831651">
+          <pm:border xmlns:pm="smNativeData" id="1627834486">
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1480,7 +1475,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1627831651">
+          <pm:border xmlns:pm="smNativeData" id="1627834486">
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1502,7 +1497,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1627831651">
+          <pm:border xmlns:pm="smNativeData" id="1627834486">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -1525,7 +1520,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1627831651">
+          <pm:border xmlns:pm="smNativeData" id="1627834486">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -1547,7 +1542,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1627831651">
+          <pm:border xmlns:pm="smNativeData" id="1627834486">
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -1557,7 +1552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1594,21 +1589,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1618,10 +1608,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1627831651" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1627834486" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1627831651" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1627834486" count="1">
         <pm:color name="Gris 20%" rgb="000000"/>
       </pm:colors>
     </ext>
@@ -1888,7 +1878,7 @@
   <dimension ref="A1:XFD624"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.553571" defaultRowHeight="15.40"/>
@@ -1896,7 +1886,7 @@
     <col min="2" max="2" width="17.553571" customWidth="1"/>
     <col min="3" max="3" width="16.107143" customWidth="1"/>
     <col min="4" max="4" width="51.330357" customWidth="1" style="8"/>
-    <col min="5" max="5" width="12.000000" customWidth="1" style="20"/>
+    <col min="5" max="5" width="12.000000" customWidth="1" style="18"/>
     <col min="6" max="6" width="10.544643" customWidth="1"/>
     <col min="7" max="7" width="36.330357" customWidth="1" style="14"/>
     <col min="9" max="9" width="18.437500" customWidth="1"/>
@@ -1917,7 +1907,7 @@
       <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="12"/>
@@ -18310,13 +18300,13 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="n">
+      <c r="B2" s="4" t="n">
         <v>246.550000000000011</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="20" t="n">
+      <c r="E2" s="18" t="n">
         <v>43678</v>
       </c>
       <c r="G2" s="14" t="s">
@@ -18327,7 +18317,7 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="n">
+      <c r="B3" s="4" t="n">
         <v>545.230000000000018</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -18341,13 +18331,13 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="n">
+      <c r="B4" s="4" t="n">
         <v>30</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="20" t="n">
+      <c r="E4" s="18" t="n">
         <v>43681</v>
       </c>
       <c r="G4" s="14" t="s">
@@ -18360,46 +18350,46 @@
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="4">
         <f>75+60</f>
         <v>135</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="20" t="n">
+      <c r="E5" s="18" t="n">
         <v>43683</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="J5"/>
+      <c r="K5"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="18" t="n">
+      <c r="B6" s="4" t="n">
         <v>16</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="20" t="n">
+      <c r="E6" s="18" t="n">
         <v>43687</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
+      <c r="J6"/>
+      <c r="K6"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="n">
+      <c r="B7" s="4" t="n">
         <v>50</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -18413,13 +18403,13 @@
       <c r="A8" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="n">
+      <c r="B8" s="4" t="n">
         <v>30</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="20" t="n">
+      <c r="E8" s="18" t="n">
         <v>43692</v>
       </c>
       <c r="G8" s="14" t="s">
@@ -18430,14 +18420,14 @@
       <c r="A9" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="n">
+      <c r="B9" s="5" t="n">
         <v>10</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="20" t="n">
+      <c r="E9" s="18" t="n">
         <v>43694</v>
       </c>
       <c r="G9" s="14" t="s">
@@ -18455,7 +18445,7 @@
       <c r="D10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="20" t="n">
+      <c r="E10" s="18" t="n">
         <v>43699</v>
       </c>
       <c r="G10" s="14" t="s">
@@ -18483,7 +18473,7 @@
       </c>
       <c r="B12" s="4"/>
       <c r="C12" t="n">
-        <v>10.3400000000000016</v>
+        <v>10.3399999999999999</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>25</v>
@@ -18533,7 +18523,7 @@
       <c r="D15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="20" t="n">
+      <c r="E15" s="18" t="n">
         <v>43700</v>
       </c>
       <c r="G15" s="14" t="s">
@@ -18686,7 +18676,7 @@
       <c r="D25" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="20" t="n">
+      <c r="E25" s="18" t="n">
         <v>43701</v>
       </c>
       <c r="G25" s="14" t="s">
@@ -18794,7 +18784,7 @@
       <c r="D32" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="20" t="n">
+      <c r="E32" s="18" t="n">
         <v>43702</v>
       </c>
       <c r="G32" s="14" t="s">
@@ -18827,7 +18817,7 @@
       <c r="D34" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="20" t="n">
+      <c r="E34" s="18" t="n">
         <v>43703</v>
       </c>
       <c r="G34" s="14" t="s">
@@ -18905,7 +18895,7 @@
       <c r="D39" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="20" t="n">
+      <c r="E39" s="18" t="n">
         <v>43704</v>
       </c>
       <c r="G39" s="14" t="s">
@@ -18968,7 +18958,7 @@
       <c r="D43" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="20" t="n">
+      <c r="E43" s="18" t="n">
         <v>43705</v>
       </c>
       <c r="G43" s="14" t="s">
@@ -19031,7 +19021,7 @@
       <c r="D47" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E47" s="20" t="n">
+      <c r="E47" s="18" t="n">
         <v>43706</v>
       </c>
       <c r="G47" s="14" t="s">
@@ -19121,7 +19111,7 @@
       <c r="D54" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E54" s="20" t="n">
+      <c r="E54" s="18" t="n">
         <v>43707</v>
       </c>
     </row>
@@ -19172,7 +19162,7 @@
       <c r="D58" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E58" s="20" t="n">
+      <c r="E58" s="18" t="n">
         <v>43708</v>
       </c>
     </row>
@@ -19207,7 +19197,7 @@
       <c r="D61" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E61" s="20" t="n">
+      <c r="E61" s="18" t="n">
         <v>43711</v>
       </c>
       <c r="G61" s="14" t="s">
@@ -19248,7 +19238,7 @@
       <c r="D64" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E64" s="20" t="n">
+      <c r="E64" s="18" t="n">
         <v>43713</v>
       </c>
       <c r="G64" s="14" t="s">
@@ -19274,7 +19264,7 @@
       <c r="D66" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E66" s="20" t="n">
+      <c r="E66" s="18" t="n">
         <v>43714</v>
       </c>
       <c r="G66" s="14" t="s">
@@ -19342,7 +19332,7 @@
       <c r="D71" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E71" s="20" t="n">
+      <c r="E71" s="18" t="n">
         <v>43715</v>
       </c>
       <c r="G71" s="14" t="s">
@@ -19368,7 +19358,7 @@
       <c r="D73" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E73" s="20" t="n">
+      <c r="E73" s="18" t="n">
         <v>43716</v>
       </c>
       <c r="G73" s="14" t="s">
@@ -19409,7 +19399,7 @@
       <c r="D76" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E76" s="20" t="n">
+      <c r="E76" s="18" t="n">
         <v>43717</v>
       </c>
       <c r="G76" s="14" t="s">
@@ -19458,7 +19448,7 @@
       <c r="D80" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E80" s="20" t="n">
+      <c r="E80" s="18" t="n">
         <v>43719</v>
       </c>
     </row>
@@ -19517,7 +19507,7 @@
       <c r="D85" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E85" s="20" t="n">
+      <c r="E85" s="18" t="n">
         <v>43720</v>
       </c>
     </row>
@@ -19540,7 +19530,7 @@
       <c r="D87" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E87" s="20" t="n">
+      <c r="E87" s="18" t="n">
         <v>43721</v>
       </c>
       <c r="G87" s="14" t="s">
@@ -19628,7 +19618,7 @@
       </c>
       <c r="B93" s="4"/>
       <c r="C93" t="n">
-        <v>13.9200000000000017</v>
+        <v>13.9199999999999999</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>103</v>
@@ -19656,7 +19646,7 @@
       <c r="D95" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="E95" s="20" t="n">
+      <c r="E95" s="18" t="n">
         <v>43723</v>
       </c>
       <c r="G95" s="14" t="s">
@@ -19697,7 +19687,7 @@
       <c r="D98" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E98" s="20" t="n">
+      <c r="E98" s="18" t="n">
         <v>43725</v>
       </c>
       <c r="G98" s="14" t="s">
@@ -19738,7 +19728,7 @@
       <c r="D101" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E101" s="20" t="n">
+      <c r="E101" s="18" t="n">
         <v>43726</v>
       </c>
       <c r="G101" s="14" t="s">
@@ -19764,7 +19754,7 @@
       <c r="D103" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="E103" s="20" t="n">
+      <c r="E103" s="18" t="n">
         <v>43727</v>
       </c>
       <c r="G103" s="14" t="s">
@@ -19790,7 +19780,7 @@
       <c r="D105" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E105" s="20" t="n">
+      <c r="E105" s="18" t="n">
         <v>43728</v>
       </c>
       <c r="G105" s="14" t="s">
@@ -19876,7 +19866,7 @@
       <c r="D111" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E111" s="20" t="n">
+      <c r="E111" s="18" t="n">
         <v>43729</v>
       </c>
       <c r="G111" s="14" t="s">
@@ -19912,12 +19902,12 @@
       </c>
       <c r="B114" s="2"/>
       <c r="C114" s="3" t="n">
-        <v>10.3400000000000016</v>
+        <v>10.3399999999999999</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E114" s="20" t="n">
+      <c r="E114" s="18" t="n">
         <v>43731</v>
       </c>
       <c r="G114" s="14" t="s">
@@ -20000,7 +19990,7 @@
       <c r="D120" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="E120" s="20" t="n">
+      <c r="E120" s="18" t="n">
         <v>43733</v>
       </c>
       <c r="G120" s="14" t="s">
@@ -20055,7 +20045,6 @@
       </c>
       <c r="B124" s="5"/>
       <c r="C124" s="1"/>
-      <c r="D124" s="22"/>
     </row>
     <row r="125" spans="1:7">
       <c r="A125" t="n">
@@ -20065,10 +20054,10 @@
       <c r="C125" s="3" t="n">
         <v>35.0200000000000031</v>
       </c>
-      <c r="D125" s="23" t="s">
+      <c r="D125" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="E125" s="20" t="n">
+      <c r="E125" s="18" t="n">
         <v>43734</v>
       </c>
       <c r="G125" s="14" t="s">
@@ -20098,7 +20087,7 @@
       <c r="C127" t="n">
         <v>23.6799999999999997</v>
       </c>
-      <c r="D127" s="22" t="s">
+      <c r="D127" s="8" t="s">
         <v>135</v>
       </c>
       <c r="G127" s="14" t="s">
@@ -20116,7 +20105,7 @@
       <c r="D128" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F128" s="20"/>
+      <c r="F128"/>
       <c r="G128" s="14" t="s">
         <v>138</v>
       </c>
@@ -20155,7 +20144,7 @@
       <c r="D131" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E131" s="20" t="n">
+      <c r="E131" s="18" t="n">
         <v>43735</v>
       </c>
       <c r="G131" s="14" t="s">
@@ -20181,7 +20170,7 @@
       <c r="D133" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="E133" s="20" t="n">
+      <c r="E133" s="18" t="n">
         <v>43737</v>
       </c>
       <c r="G133" s="14" t="s">
@@ -20207,7 +20196,7 @@
       <c r="D135" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="E135" s="20" t="n">
+      <c r="E135" s="18" t="n">
         <v>43738</v>
       </c>
       <c r="G135" s="14" t="s">
@@ -20257,7 +20246,7 @@
       <c r="D139" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E139" s="20" t="n">
+      <c r="E139" s="18" t="n">
         <v>43741</v>
       </c>
       <c r="G139" s="14" t="s">
@@ -20298,7 +20287,7 @@
       <c r="D142" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="E142" s="20" t="n">
+      <c r="E142" s="18" t="n">
         <v>43742</v>
       </c>
       <c r="G142" s="14" t="s">
@@ -20339,7 +20328,7 @@
       <c r="D145" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="E145" s="20" t="n">
+      <c r="E145" s="18" t="n">
         <v>43743</v>
       </c>
       <c r="G145" s="14" t="s">
@@ -20380,7 +20369,7 @@
       <c r="D148" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="E148" s="20" t="n">
+      <c r="E148" s="18" t="n">
         <v>43747</v>
       </c>
       <c r="G148" s="14" t="s">
@@ -20406,7 +20395,7 @@
       <c r="D150" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="E150" s="20" t="n">
+      <c r="E150" s="18" t="n">
         <v>43748</v>
       </c>
       <c r="G150" s="14" t="s">
@@ -20478,7 +20467,7 @@
       <c r="D155" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="E155" s="20" t="n">
+      <c r="E155" s="18" t="n">
         <v>43749</v>
       </c>
       <c r="G155" s="14" t="s">
@@ -20547,7 +20536,7 @@
       <c r="D160" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E160" s="20" t="n">
+      <c r="E160" s="18" t="n">
         <v>43750</v>
       </c>
       <c r="G160" s="14" t="s">
@@ -20573,7 +20562,7 @@
       <c r="D162" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="E162" s="20" t="n">
+      <c r="E162" s="18" t="n">
         <v>43751</v>
       </c>
       <c r="G162" s="14" t="s">
@@ -20599,7 +20588,7 @@
       <c r="D164" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E164" s="20" t="n">
+      <c r="E164" s="18" t="n">
         <v>43752</v>
       </c>
       <c r="G164" s="14" t="s">
@@ -20640,7 +20629,7 @@
       <c r="D167" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E167" s="20" t="n">
+      <c r="E167" s="18" t="n">
         <v>43754</v>
       </c>
       <c r="G167" s="14" t="s">
@@ -20679,7 +20668,7 @@
       <c r="D170" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="E170" s="20" t="n">
+      <c r="E170" s="18" t="n">
         <v>43756</v>
       </c>
       <c r="G170" s="14" t="s">
@@ -20758,7 +20747,7 @@
       <c r="D175" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="E175" s="20" t="n">
+      <c r="E175" s="18" t="n">
         <v>43757</v>
       </c>
       <c r="G175" s="14" t="s">
@@ -20855,7 +20844,7 @@
       <c r="D181" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="E181" s="20" t="n">
+      <c r="E181" s="18" t="n">
         <v>43758</v>
       </c>
       <c r="G181" s="14" t="s">
@@ -20918,7 +20907,7 @@
       <c r="D185" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="E185" s="20" t="n">
+      <c r="E185" s="18" t="n">
         <v>43759</v>
       </c>
       <c r="G185" s="14" t="s">
@@ -20958,7 +20947,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="4"/>
-      <c r="E188" s="20" t="n">
+      <c r="E188" s="18" t="n">
         <v>43760</v>
       </c>
     </row>
@@ -20996,7 +20985,7 @@
       <c r="D191" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="E191" s="20" t="n">
+      <c r="E191" s="18" t="n">
         <v>43761</v>
       </c>
       <c r="G191" s="14" t="s">
@@ -21037,7 +21026,7 @@
       <c r="D194" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E194" s="20" t="n">
+      <c r="E194" s="18" t="n">
         <v>43763</v>
       </c>
       <c r="G194" s="14" t="s">
@@ -21082,7 +21071,7 @@
       <c r="D198" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E198" s="20" t="n">
+      <c r="E198" s="18" t="n">
         <v>43765</v>
       </c>
       <c r="G198" s="14" t="s">
@@ -21104,7 +21093,7 @@
       <c r="D200" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="E200" s="20" t="n">
+      <c r="E200" s="18" t="n">
         <v>43766</v>
       </c>
       <c r="G200" s="14" t="s">
@@ -21128,7 +21117,7 @@
       <c r="A203" t="n">
         <v>202</v>
       </c>
-      <c r="E203" s="20" t="n">
+      <c r="E203" s="18" t="n">
         <v>43767</v>
       </c>
     </row>
@@ -21148,7 +21137,7 @@
       <c r="D205" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="E205" s="20" t="n">
+      <c r="E205" s="18" t="n">
         <v>43768</v>
       </c>
       <c r="G205" s="14" t="s">
@@ -21177,7 +21166,7 @@
       <c r="D207" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="E207" s="20" t="n">
+      <c r="E207" s="18" t="n">
         <v>43769</v>
       </c>
       <c r="G207" s="14" t="s">
@@ -21206,7 +21195,7 @@
       <c r="D209" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="E209" s="20" t="n">
+      <c r="E209" s="18" t="n">
         <v>43770</v>
       </c>
       <c r="G209" s="14" t="s">
@@ -21235,7 +21224,7 @@
       <c r="D211" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="E211" s="20" t="n">
+      <c r="E211" s="18" t="n">
         <v>43773</v>
       </c>
       <c r="G211" s="14" t="s">
@@ -21264,7 +21253,7 @@
       <c r="D213" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="E213" s="20" t="n">
+      <c r="E213" s="18" t="n">
         <v>43774</v>
       </c>
       <c r="G213" s="14" t="s">
@@ -21304,7 +21293,7 @@
       <c r="D216" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="E216" s="20" t="n">
+      <c r="E216" s="18" t="n">
         <v>43775</v>
       </c>
       <c r="G216" s="14" t="s">
@@ -21345,7 +21334,7 @@
       <c r="D219" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="E219" s="20" t="n">
+      <c r="E219" s="18" t="n">
         <v>43777</v>
       </c>
       <c r="G219" s="14" t="s">
@@ -21371,7 +21360,7 @@
       <c r="D221" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E221" s="20" t="n">
+      <c r="E221" s="18" t="n">
         <v>43778</v>
       </c>
       <c r="G221" s="14" t="s">
@@ -21397,7 +21386,7 @@
       <c r="D223" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="E223" s="20" t="n">
+      <c r="E223" s="18" t="n">
         <v>43784</v>
       </c>
       <c r="G223" s="14" t="s">
@@ -21468,7 +21457,7 @@
       <c r="D228" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="E228" s="20" t="n">
+      <c r="E228" s="18" t="n">
         <v>43785</v>
       </c>
       <c r="G228" s="14" t="s">
@@ -21509,7 +21498,7 @@
       <c r="D231" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="E231" s="20" t="n">
+      <c r="E231" s="18" t="n">
         <v>43786</v>
       </c>
       <c r="G231" s="14" t="s">
@@ -21565,7 +21554,7 @@
       <c r="D235" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="E235" s="20" t="n">
+      <c r="E235" s="18" t="n">
         <v>43791</v>
       </c>
       <c r="G235" s="14" t="s">
@@ -21648,7 +21637,7 @@
       <c r="D240" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="E240" s="20" t="n">
+      <c r="E240" s="18" t="n">
         <v>43797</v>
       </c>
       <c r="G240" s="14" t="s">
@@ -21733,7 +21722,7 @@
       <c r="D246" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="E246" s="20" t="n">
+      <c r="E246" s="18" t="n">
         <v>43798</v>
       </c>
       <c r="G246" s="14" t="s">
@@ -21780,7 +21769,7 @@
       <c r="D250" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="E250" s="20" t="n">
+      <c r="E250" s="18" t="n">
         <v>43800</v>
       </c>
       <c r="G250" s="14" t="s">
@@ -21806,7 +21795,7 @@
       <c r="D252" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="E252" s="20" t="n">
+      <c r="E252" s="18" t="n">
         <v>43802</v>
       </c>
       <c r="G252" s="14" t="s">
@@ -21847,7 +21836,7 @@
       <c r="D255" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="E255" s="20" t="n">
+      <c r="E255" s="18" t="n">
         <v>43804</v>
       </c>
       <c r="G255" s="14" t="s">
@@ -21903,7 +21892,7 @@
       <c r="D259" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="E259" s="20" t="n">
+      <c r="E259" s="18" t="n">
         <v>43808</v>
       </c>
       <c r="G259" s="14" t="s">
@@ -21929,7 +21918,7 @@
       <c r="D261" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="E261" s="20" t="n">
+      <c r="E261" s="18" t="n">
         <v>43809</v>
       </c>
       <c r="G261" s="14" t="s">
@@ -21953,7 +21942,7 @@
       <c r="D263" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E263" s="20" t="n">
+      <c r="E263" s="18" t="n">
         <v>43811</v>
       </c>
       <c r="G263" s="14" t="s">
@@ -22002,12 +21991,12 @@
       </c>
       <c r="B267" s="2"/>
       <c r="C267" s="3" t="n">
-        <v>11.4200000000000017</v>
+        <v>11.4199999999999999</v>
       </c>
       <c r="D267" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="E267" s="20" t="n">
+      <c r="E267" s="18" t="n">
         <v>43814</v>
       </c>
       <c r="G267" s="14" t="s">
@@ -22046,7 +22035,7 @@
       <c r="D270" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="E270" s="20" t="n">
+      <c r="E270" s="18" t="n">
         <v>43815</v>
       </c>
       <c r="G270" s="14" t="s">
@@ -22115,7 +22104,7 @@
       <c r="D275" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="E275" s="20" t="n">
+      <c r="E275" s="18" t="n">
         <v>43816</v>
       </c>
       <c r="G275" s="14" t="s">
@@ -22139,7 +22128,7 @@
       <c r="D277" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="E277" s="20" t="n">
+      <c r="E277" s="18" t="n">
         <v>43817</v>
       </c>
       <c r="G277" s="14" t="s">
@@ -22163,7 +22152,7 @@
       <c r="D279" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="E279" s="20" t="n">
+      <c r="E279" s="18" t="n">
         <v>43818</v>
       </c>
       <c r="G279" s="14" t="s">
@@ -22217,7 +22206,7 @@
       <c r="D283" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="E283" s="20" t="n">
+      <c r="E283" s="18" t="n">
         <v>43821</v>
       </c>
       <c r="G283" s="14" t="s">
@@ -22304,7 +22293,7 @@
       <c r="D289" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="E289" s="20" t="n">
+      <c r="E289" s="18" t="n">
         <v>43824</v>
       </c>
       <c r="G289" s="14" t="s">
@@ -22360,7 +22349,7 @@
       <c r="D293" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="E293" s="20" t="n">
+      <c r="E293" s="18" t="n">
         <v>43825</v>
       </c>
       <c r="G293" s="14" t="s">
@@ -22429,7 +22418,7 @@
       <c r="D298" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="E298" s="20" t="n">
+      <c r="E298" s="18" t="n">
         <v>43830</v>
       </c>
       <c r="G298" s="14" t="s">
@@ -22469,7 +22458,7 @@
       <c r="D301" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="E301" s="20" t="n">
+      <c r="E301" s="18" t="n">
         <v>43831</v>
       </c>
       <c r="G301" s="14" t="s">
@@ -22496,7 +22485,7 @@
       <c r="D303" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E303" s="20" t="n">
+      <c r="E303" s="18" t="n">
         <v>43835</v>
       </c>
       <c r="G303" s="8" t="s">
@@ -22520,10 +22509,10 @@
       <c r="D305" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="E305" s="20" t="n">
+      <c r="E305" s="18" t="n">
         <v>43838</v>
       </c>
-      <c r="G305" s="22" t="s">
+      <c r="G305" s="8" t="s">
         <v>86</v>
       </c>
     </row>
@@ -22545,7 +22534,7 @@
       <c r="D307" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="E307" s="20" t="n">
+      <c r="E307" s="18" t="n">
         <v>43839</v>
       </c>
       <c r="G307" s="14" t="s">
@@ -22563,7 +22552,7 @@
       <c r="D308" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="E308" s="22"/>
+      <c r="E308" s="20"/>
       <c r="G308" s="14" t="s">
         <v>159</v>
       </c>
@@ -22586,7 +22575,7 @@
       <c r="D310" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E310" s="20" t="n">
+      <c r="E310" s="18" t="n">
         <v>43840</v>
       </c>
       <c r="G310" s="14" t="s">
@@ -22610,7 +22599,7 @@
       <c r="D312" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="E312" s="20" t="n">
+      <c r="E312" s="18" t="n">
         <v>43841</v>
       </c>
       <c r="G312" s="14" t="s">
@@ -22637,7 +22626,7 @@
       <c r="D314" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E314" s="20" t="n">
+      <c r="E314" s="18" t="n">
         <v>43844</v>
       </c>
       <c r="G314" s="14" t="s">
@@ -22661,7 +22650,7 @@
       <c r="D316" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="E316" s="20" t="n">
+      <c r="E316" s="18" t="n">
         <v>43845</v>
       </c>
       <c r="G316" s="14" t="s">
@@ -22703,7 +22692,7 @@
       <c r="D319" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="E319" s="20" t="n">
+      <c r="E319" s="18" t="n">
         <v>43846</v>
       </c>
       <c r="G319" s="14" t="s">
@@ -22745,7 +22734,7 @@
       <c r="D322" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="E322" s="20" t="n">
+      <c r="E322" s="18" t="n">
         <v>43848</v>
       </c>
       <c r="G322" s="14" t="s">
@@ -22769,7 +22758,7 @@
       <c r="D324" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="E324" s="20" t="n">
+      <c r="E324" s="18" t="n">
         <v>43850</v>
       </c>
       <c r="G324" s="14" t="s">
@@ -22808,7 +22797,7 @@
       <c r="D327" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="E327" s="20" t="n">
+      <c r="E327" s="18" t="n">
         <v>43855</v>
       </c>
       <c r="G327" s="14" t="s">
@@ -22847,7 +22836,7 @@
       <c r="D330" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="E330" s="20" t="n">
+      <c r="E330" s="18" t="n">
         <v>43856</v>
       </c>
       <c r="G330" s="14" t="s">
@@ -22901,7 +22890,7 @@
       <c r="D334" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="E334" s="20" t="n">
+      <c r="E334" s="18" t="n">
         <v>43859</v>
       </c>
       <c r="G334" s="14" t="s">
@@ -22925,7 +22914,7 @@
       <c r="D336" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="E336" s="20" t="n">
+      <c r="E336" s="18" t="n">
         <v>43860</v>
       </c>
       <c r="G336" s="14" t="s">
@@ -22964,7 +22953,7 @@
       <c r="D339" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="E339" s="20" t="n">
+      <c r="E339" s="18" t="n">
         <v>43863</v>
       </c>
     </row>
@@ -22997,7 +22986,7 @@
       <c r="D342" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="E342" s="20" t="n">
+      <c r="E342" s="18" t="n">
         <v>43864</v>
       </c>
     </row>
@@ -23018,7 +23007,7 @@
       <c r="D344" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="E344" s="20" t="n">
+      <c r="E344" s="18" t="n">
         <v>43865</v>
       </c>
     </row>
@@ -23039,7 +23028,7 @@
       <c r="D346" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="E346" s="20" t="n">
+      <c r="E346" s="18" t="n">
         <v>43866</v>
       </c>
       <c r="G346" s="14" t="s">
@@ -23063,7 +23052,7 @@
       <c r="D348" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="E348" s="20" t="n">
+      <c r="E348" s="18" t="n">
         <v>43867</v>
       </c>
       <c r="G348" s="14" t="s">
@@ -23124,7 +23113,7 @@
       <c r="D352" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="E352" s="20" t="n">
+      <c r="E352" s="18" t="n">
         <v>43868</v>
       </c>
       <c r="G352" s="14" t="s">
@@ -23168,7 +23157,7 @@
       <c r="D355" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="E355" s="20" t="n">
+      <c r="E355" s="18" t="n">
         <v>43869</v>
       </c>
       <c r="G355" s="14" t="s">
@@ -23195,7 +23184,7 @@
       <c r="D357" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="E357" s="20" t="n">
+      <c r="E357" s="18" t="n">
         <v>43870</v>
       </c>
       <c r="G357" s="14" t="s">
@@ -23239,7 +23228,7 @@
       <c r="D360" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E360" s="20" t="n">
+      <c r="E360" s="18" t="n">
         <v>43871</v>
       </c>
       <c r="G360" s="14" t="s">
@@ -23266,7 +23255,7 @@
       <c r="D362" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="E362" s="20" t="n">
+      <c r="E362" s="18" t="n">
         <v>43873</v>
       </c>
       <c r="G362" s="14" t="s">
@@ -23290,7 +23279,7 @@
       <c r="D364" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="E364" s="20" t="n">
+      <c r="E364" s="18" t="n">
         <v>43874</v>
       </c>
       <c r="G364" s="14" t="s">
@@ -23314,7 +23303,7 @@
       <c r="D366" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E366" s="20" t="n">
+      <c r="E366" s="18" t="n">
         <v>43875</v>
       </c>
       <c r="G366" s="14" t="s">
@@ -23338,7 +23327,7 @@
       <c r="D368" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E368" s="20" t="n">
+      <c r="E368" s="18" t="n">
         <v>43876</v>
       </c>
       <c r="G368" s="14" t="s">
@@ -23377,7 +23366,7 @@
       <c r="D371" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E371" s="20" t="n">
+      <c r="E371" s="18" t="n">
         <v>43878</v>
       </c>
       <c r="G371" s="14" t="s">
@@ -23401,7 +23390,7 @@
       <c r="D373" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="E373" s="20" t="n">
+      <c r="E373" s="18" t="n">
         <v>43880</v>
       </c>
       <c r="G373" s="14" t="s">
@@ -23425,7 +23414,7 @@
       <c r="D375" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="E375" s="20" t="n">
+      <c r="E375" s="18" t="n">
         <v>43887</v>
       </c>
       <c r="G375" s="14" t="s">
@@ -23464,7 +23453,7 @@
       <c r="D378" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="E378" s="20" t="n">
+      <c r="E378" s="18" t="n">
         <v>43888</v>
       </c>
       <c r="G378" s="14" t="s">
@@ -23488,7 +23477,7 @@
       <c r="D380" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="E380" s="20" t="n">
+      <c r="E380" s="18" t="n">
         <v>43890</v>
       </c>
       <c r="G380" s="14" t="s">
@@ -23512,7 +23501,7 @@
       <c r="D382" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="E382" s="20" t="n">
+      <c r="E382" s="18" t="n">
         <v>43891</v>
       </c>
       <c r="G382" s="14" t="s">
@@ -23536,7 +23525,7 @@
       <c r="D384" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E384" s="20" t="n">
+      <c r="E384" s="18" t="n">
         <v>43892</v>
       </c>
       <c r="G384" s="14" t="s">
@@ -23605,7 +23594,7 @@
       <c r="D389" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="E389" s="20" t="n">
+      <c r="E389" s="18" t="n">
         <v>43894</v>
       </c>
       <c r="G389" s="14" t="s">
@@ -23685,7 +23674,7 @@
       <c r="D394" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="E394" s="20" t="n">
+      <c r="E394" s="18" t="n">
         <v>43895</v>
       </c>
       <c r="G394" s="14" t="s">
@@ -23739,7 +23728,7 @@
       <c r="D397" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="E397" s="20" t="n">
+      <c r="E397" s="18" t="n">
         <v>43896</v>
       </c>
       <c r="G397" s="14" t="s">
@@ -23784,7 +23773,7 @@
       <c r="D400" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="E400" s="20" t="n">
+      <c r="E400" s="18" t="n">
         <v>43897</v>
       </c>
       <c r="G400" s="14" t="s">
@@ -23811,7 +23800,7 @@
       <c r="D402" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="E402" s="20" t="n">
+      <c r="E402" s="18" t="n">
         <v>43898</v>
       </c>
       <c r="G402" s="14" t="s">
@@ -23838,7 +23827,7 @@
       <c r="D404" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="E404" s="20" t="n">
+      <c r="E404" s="18" t="n">
         <v>43900</v>
       </c>
       <c r="G404" s="14" t="s">
@@ -23877,7 +23866,7 @@
       <c r="D407" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="E407" s="20" t="n">
+      <c r="E407" s="18" t="n">
         <v>43901</v>
       </c>
       <c r="G407" s="14" t="s">
@@ -23931,7 +23920,7 @@
       <c r="D411" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="E411" s="20" t="n">
+      <c r="E411" s="18" t="n">
         <v>43903</v>
       </c>
       <c r="G411" s="14" t="s">
@@ -23958,7 +23947,7 @@
       <c r="D413" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="E413" s="20" t="n">
+      <c r="E413" s="18" t="n">
         <v>43904</v>
       </c>
       <c r="G413" s="14" t="s">
@@ -24019,7 +24008,7 @@
       <c r="D417" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="E417" s="20" t="n">
+      <c r="E417" s="18" t="n">
         <v>43905</v>
       </c>
       <c r="G417" s="14" t="s">
@@ -24080,7 +24069,7 @@
       <c r="D421" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="E421" s="20" t="n">
+      <c r="E421" s="18" t="n">
         <v>43906</v>
       </c>
       <c r="G421" s="14" t="s">
@@ -24114,7 +24103,7 @@
       <c r="D424" s="9" t="s">
         <v>331</v>
       </c>
-      <c r="E424" s="20" t="n">
+      <c r="E424" s="18" t="n">
         <v>43907</v>
       </c>
       <c r="G424" s="14" t="s">
@@ -24165,7 +24154,7 @@
       <c r="D428" s="9" t="s">
         <v>334</v>
       </c>
-      <c r="E428" s="20" t="n">
+      <c r="E428" s="18" t="n">
         <v>43908</v>
       </c>
       <c r="G428" s="14" t="s">
@@ -24192,7 +24181,7 @@
       <c r="D430" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="E430" s="20" t="n">
+      <c r="E430" s="18" t="n">
         <v>43910</v>
       </c>
       <c r="G430" s="14" t="s">
@@ -24211,12 +24200,12 @@
       </c>
       <c r="B432" s="2"/>
       <c r="C432" s="3" t="n">
-        <v>114.110000000000014</v>
+        <v>114.109999999999999</v>
       </c>
       <c r="D432" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E432" s="20" t="n">
+      <c r="E432" s="18" t="n">
         <v>43912</v>
       </c>
       <c r="G432" s="14" t="s">
@@ -24241,7 +24230,7 @@
       <c r="D434" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="E434" s="20" t="n">
+      <c r="E434" s="18" t="n">
         <v>43913</v>
       </c>
       <c r="G434" s="14" t="s">
@@ -24279,7 +24268,7 @@
       <c r="D437" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="E437" s="20" t="n">
+      <c r="E437" s="18" t="n">
         <v>43923</v>
       </c>
       <c r="G437" s="14" t="s">
@@ -24303,7 +24292,7 @@
       <c r="D439" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E439" s="20" t="n">
+      <c r="E439" s="18" t="n">
         <v>43924</v>
       </c>
       <c r="G439" s="14" t="s">
@@ -24327,7 +24316,7 @@
       <c r="D441" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E441" s="20" t="n">
+      <c r="E441" s="18" t="n">
         <v>43935</v>
       </c>
       <c r="G441" s="14" t="s">
@@ -24351,7 +24340,7 @@
       <c r="D443" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="E443" s="20" t="n">
+      <c r="E443" s="18" t="n">
         <v>43938</v>
       </c>
       <c r="G443" s="14" t="s">
@@ -24375,7 +24364,7 @@
       <c r="D445" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E445" s="20" t="n">
+      <c r="E445" s="18" t="n">
         <v>43939</v>
       </c>
       <c r="G445" s="14" t="s">
@@ -24399,7 +24388,7 @@
       <c r="D447" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E447" s="20" t="n">
+      <c r="E447" s="18" t="n">
         <v>43948</v>
       </c>
       <c r="G447" s="14" t="s">
@@ -24439,7 +24428,7 @@
       <c r="D450" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E450" s="20" t="n">
+      <c r="E450" s="18" t="n">
         <v>43958</v>
       </c>
       <c r="G450" s="14" t="s">
@@ -24461,7 +24450,7 @@
       <c r="D452" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="E452" s="20" t="n">
+      <c r="E452" s="18" t="n">
         <v>43960</v>
       </c>
       <c r="G452" s="14" t="s">
@@ -24483,7 +24472,7 @@
       <c r="D454" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E454" s="20" t="n">
+      <c r="E454" s="18" t="n">
         <v>43964</v>
       </c>
       <c r="G454" s="14" t="s">
@@ -24505,7 +24494,7 @@
       <c r="D456" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="E456" s="20" t="n">
+      <c r="E456" s="18" t="n">
         <v>43966</v>
       </c>
       <c r="G456" s="14" t="s">
@@ -24541,7 +24530,7 @@
       <c r="D459" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="E459" s="20" t="n">
+      <c r="E459" s="18" t="n">
         <v>43967</v>
       </c>
       <c r="G459" s="14" t="s">
@@ -24563,7 +24552,7 @@
       <c r="D461" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="E461" s="20" t="n">
+      <c r="E461" s="18" t="n">
         <v>43971</v>
       </c>
       <c r="G461" s="14" t="s">
@@ -24585,7 +24574,7 @@
       <c r="D463" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E463" s="20" t="n">
+      <c r="E463" s="18" t="n">
         <v>43973</v>
       </c>
       <c r="G463" s="14" t="s">
@@ -24607,7 +24596,7 @@
       <c r="D465" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="E465" s="20" t="n">
+      <c r="E465" s="18" t="n">
         <v>43979</v>
       </c>
       <c r="G465" s="14" t="s">
@@ -24657,7 +24646,7 @@
       <c r="D469" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="E469" s="20" t="n">
+      <c r="E469" s="18" t="n">
         <v>43984</v>
       </c>
       <c r="G469" s="14" t="s">
@@ -24679,7 +24668,7 @@
       <c r="D471" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E471" s="20" t="n">
+      <c r="E471" s="18" t="n">
         <v>43985</v>
       </c>
       <c r="G471" s="14" t="s">
@@ -24729,7 +24718,7 @@
       <c r="D475" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="E475" s="20" t="n">
+      <c r="E475" s="18" t="n">
         <v>43986</v>
       </c>
       <c r="G475" s="14" t="s">
@@ -24751,7 +24740,7 @@
       <c r="D477" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="E477" s="20" t="n">
+      <c r="E477" s="18" t="n">
         <v>43987</v>
       </c>
       <c r="G477" s="14" t="s">
@@ -24773,7 +24762,7 @@
       <c r="D479" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E479" s="20" t="n">
+      <c r="E479" s="18" t="n">
         <v>43990</v>
       </c>
     </row>
@@ -24792,7 +24781,7 @@
       <c r="D481" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="E481" s="20" t="n">
+      <c r="E481" s="18" t="n">
         <v>43992</v>
       </c>
       <c r="G481" s="14" t="s">
@@ -24814,7 +24803,7 @@
       <c r="D483" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E483" s="20" t="n">
+      <c r="E483" s="18" t="n">
         <v>43994</v>
       </c>
     </row>
@@ -24847,7 +24836,7 @@
       <c r="D486" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E486" s="20" t="n">
+      <c r="E486" s="18" t="n">
         <v>43995</v>
       </c>
     </row>
@@ -24866,7 +24855,7 @@
       <c r="D488" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E488" s="20" t="n">
+      <c r="E488" s="18" t="n">
         <v>43996</v>
       </c>
     </row>
@@ -24885,7 +24874,7 @@
       <c r="D490" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="E490" s="20" t="n">
+      <c r="E490" s="18" t="n">
         <v>43997</v>
       </c>
       <c r="G490" s="14" t="s">
@@ -24907,7 +24896,7 @@
       <c r="D492" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="E492" s="20" t="n">
+      <c r="E492" s="18" t="n">
         <v>43998</v>
       </c>
       <c r="G492" s="14" t="s">
@@ -24943,7 +24932,7 @@
       <c r="D495" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="E495" s="20" t="n">
+      <c r="E495" s="18" t="n">
         <v>43999</v>
       </c>
       <c r="G495" s="14" t="s">
@@ -24965,7 +24954,7 @@
       <c r="D497" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="E497" s="20" t="n">
+      <c r="E497" s="18" t="n">
         <v>44000</v>
       </c>
     </row>
@@ -24984,7 +24973,7 @@
       <c r="D499" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="E499" s="20" t="n">
+      <c r="E499" s="18" t="n">
         <v>44004</v>
       </c>
       <c r="G499" s="14" t="s">
@@ -25020,7 +25009,7 @@
       <c r="D502" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="E502" s="20" t="n">
+      <c r="E502" s="18" t="n">
         <v>44008</v>
       </c>
     </row>
@@ -25053,7 +25042,7 @@
       <c r="D505" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E505" s="20" t="n">
+      <c r="E505" s="18" t="n">
         <v>44013</v>
       </c>
       <c r="G505" s="14" t="s">
@@ -25075,7 +25064,7 @@
       <c r="D507" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="E507" s="20" t="n">
+      <c r="E507" s="18" t="n">
         <v>44015</v>
       </c>
       <c r="G507" s="14" t="s">
@@ -25097,7 +25086,7 @@
       <c r="D509" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E509" s="20" t="n">
+      <c r="E509" s="18" t="n">
         <v>44016</v>
       </c>
       <c r="G509" s="14" t="s">
@@ -25130,7 +25119,7 @@
       <c r="D512" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="E512" s="20" t="n">
+      <c r="E512" s="18" t="n">
         <v>44019</v>
       </c>
       <c r="G512" s="14" t="s">
@@ -25166,7 +25155,7 @@
       <c r="D515" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="E515" s="20" t="n">
+      <c r="E515" s="18" t="n">
         <v>44020</v>
       </c>
       <c r="G515" s="14" t="s">
@@ -25216,7 +25205,7 @@
       <c r="D519" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="E519" s="20" t="n">
+      <c r="E519" s="18" t="n">
         <v>44022</v>
       </c>
     </row>
@@ -25291,7 +25280,7 @@
       <c r="D525" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E525" s="20" t="n">
+      <c r="E525" s="18" t="n">
         <v>44026</v>
       </c>
       <c r="G525" s="14" t="s">
@@ -25313,7 +25302,7 @@
       <c r="D527" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="E527" s="20" t="n">
+      <c r="E527" s="18" t="n">
         <v>44027</v>
       </c>
       <c r="G527" s="14" t="s">
@@ -25335,7 +25324,7 @@
       <c r="D529" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="E529" s="20" t="n">
+      <c r="E529" s="18" t="n">
         <v>44028</v>
       </c>
       <c r="G529" s="14" t="s">
@@ -25385,7 +25374,7 @@
       <c r="D533" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="E533" s="20" t="n">
+      <c r="E533" s="18" t="n">
         <v>44031</v>
       </c>
       <c r="G533" s="14" t="s">
@@ -25435,7 +25424,7 @@
       <c r="D537" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="E537" s="20" t="n">
+      <c r="E537" s="18" t="n">
         <v>44032</v>
       </c>
       <c r="G537" s="14" t="s">
@@ -25482,7 +25471,7 @@
       <c r="D541" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="E541" s="20" t="n">
+      <c r="E541" s="18" t="n">
         <v>44033</v>
       </c>
       <c r="G541" s="14" t="s">
@@ -25515,7 +25504,7 @@
       <c r="D544" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="E544" s="20" t="n">
+      <c r="E544" s="18" t="n">
         <v>44034</v>
       </c>
       <c r="G544" s="14" t="s">
@@ -25537,7 +25526,7 @@
       <c r="D546" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E546" s="20" t="n">
+      <c r="E546" s="18" t="n">
         <v>44036</v>
       </c>
     </row>
@@ -25556,7 +25545,7 @@
       <c r="D548" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="E548" s="20" t="n">
+      <c r="E548" s="18" t="n">
         <v>44037</v>
       </c>
       <c r="G548" s="14" t="s">
@@ -25578,7 +25567,7 @@
       <c r="D550" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="E550" s="20" t="n">
+      <c r="E550" s="18" t="n">
         <v>44040</v>
       </c>
       <c r="G550" s="14" t="s">
@@ -25600,7 +25589,7 @@
       <c r="D552" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="E552" s="20" t="n">
+      <c r="E552" s="18" t="n">
         <v>44041</v>
       </c>
       <c r="G552" s="14" t="s">
@@ -25695,7 +25684,7 @@
       <c r="D559" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="E559" s="20" t="n">
+      <c r="E559" s="18" t="n">
         <v>44042</v>
       </c>
       <c r="G559" s="14" t="s">
@@ -25745,7 +25734,7 @@
       <c r="D563" s="16" t="s">
         <v>389</v>
       </c>
-      <c r="E563" s="24" t="n">
+      <c r="E563" s="21" t="n">
         <v>44046</v>
       </c>
       <c r="F563" s="16"/>
@@ -25763,7 +25752,7 @@
       <c r="D564" s="16" t="s">
         <v>378</v>
       </c>
-      <c r="E564" s="25"/>
+      <c r="E564" s="22"/>
       <c r="F564" s="16"/>
       <c r="G564" s="16" t="s">
         <v>73</v>
@@ -25779,7 +25768,7 @@
       <c r="D565" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="E565" s="25"/>
+      <c r="E565" s="22"/>
       <c r="F565" s="16"/>
       <c r="G565" s="16"/>
     </row>
@@ -25789,7 +25778,7 @@
       </c>
       <c r="C566" s="16"/>
       <c r="D566" s="16"/>
-      <c r="E566" s="25"/>
+      <c r="E566" s="22"/>
       <c r="F566" s="16"/>
       <c r="G566" s="16"/>
     </row>
@@ -25803,7 +25792,7 @@
       <c r="D567" s="16" t="s">
         <v>391</v>
       </c>
-      <c r="E567" s="26" t="n">
+      <c r="E567" s="23" t="n">
         <v>44050</v>
       </c>
       <c r="F567" s="16"/>
@@ -25817,7 +25806,7 @@
       </c>
       <c r="C568" s="16"/>
       <c r="D568" s="16"/>
-      <c r="E568" s="25"/>
+      <c r="E568" s="22"/>
       <c r="F568" s="16"/>
       <c r="G568" s="16"/>
     </row>
@@ -25831,7 +25820,7 @@
       <c r="D569" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="E569" s="26" t="n">
+      <c r="E569" s="23" t="n">
         <v>44051</v>
       </c>
       <c r="F569" s="16"/>
@@ -25845,7 +25834,7 @@
       </c>
       <c r="C570" s="16"/>
       <c r="D570" s="16"/>
-      <c r="E570" s="25"/>
+      <c r="E570" s="22"/>
       <c r="F570" s="16"/>
       <c r="G570" s="16"/>
     </row>
@@ -25859,7 +25848,7 @@
       <c r="D571" s="16" t="s">
         <v>393</v>
       </c>
-      <c r="E571" s="26" t="n">
+      <c r="E571" s="23" t="n">
         <v>44052</v>
       </c>
       <c r="F571" s="16"/>
@@ -25884,7 +25873,7 @@
       <c r="D573" t="s">
         <v>211</v>
       </c>
-      <c r="E573" s="20" t="n">
+      <c r="E573" s="18" t="n">
         <v>44054</v>
       </c>
       <c r="G573" s="16" t="s">
@@ -25908,7 +25897,7 @@
       <c r="D575" t="s">
         <v>211</v>
       </c>
-      <c r="E575" s="20" t="n">
+      <c r="E575" s="18" t="n">
         <v>44057</v>
       </c>
       <c r="G575" s="16" t="s">
@@ -25932,7 +25921,7 @@
       <c r="D577" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="E577" s="20" t="n">
+      <c r="E577" s="18" t="n">
         <v>44059</v>
       </c>
       <c r="G577" s="14" t="s">
@@ -25968,7 +25957,7 @@
       <c r="D580" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="E580" s="20" t="n">
+      <c r="E580" s="18" t="n">
         <v>44061</v>
       </c>
       <c r="G580" s="14" t="s">
@@ -25980,7 +25969,6 @@
         <v>580</v>
       </c>
       <c r="D581"/>
-      <c r="E581"/>
       <c r="G581"/>
     </row>
     <row r="582" spans="1:5">
@@ -25993,7 +25981,7 @@
       <c r="D582" t="s">
         <v>211</v>
       </c>
-      <c r="E582" s="20" t="n">
+      <c r="E582" s="18" t="n">
         <v>44063</v>
       </c>
     </row>
@@ -26007,7 +25995,6 @@
       <c r="D583" t="s">
         <v>92</v>
       </c>
-      <c r="E583"/>
     </row>
     <row r="584" spans="1:5">
       <c r="A584" t="n">
@@ -26019,7 +26006,7 @@
       <c r="D584" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="E584" s="20" t="n">
+      <c r="E584" s="18" t="n">
         <v>44065</v>
       </c>
     </row>
@@ -26043,7 +26030,7 @@
       <c r="D587" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="E587" s="20" t="n">
+      <c r="E587" s="18" t="n">
         <v>44068</v>
       </c>
     </row>
@@ -26068,7 +26055,7 @@
       <c r="D589" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="E589" s="20" t="n">
+      <c r="E589" s="18" t="n">
         <v>44069</v>
       </c>
     </row>
@@ -26251,7 +26238,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1627831651" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1627834486" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -26260,14 +26247,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1627831651" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1627831651" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1627834486" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1627834486" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1627831651" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1627834486" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -26289,7 +26276,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1627831651" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1627834486" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -26298,14 +26285,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1627831651" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1627831651" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1627834486" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1627834486" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1627831651" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1627834486" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -26327,7 +26314,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1627831651" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1627834486" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -26336,14 +26323,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1627831651" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1627831651" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1627834486" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1627834486" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1627831651" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1627834486" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>